<commit_message>
Add bonus to document
</commit_message>
<xml_diff>
--- a/analysis/stat_analysis.xlsx
+++ b/analysis/stat_analysis.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwlor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22BD86AA-777A-4826-9AAC-035AEC441F2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14010" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="website_puzzle" sheetId="2" r:id="rId1"/>
     <sheet name="random_gen" sheetId="1" r:id="rId2"/>
+    <sheet name="website_puzzle_bonus" sheetId="3" r:id="rId3"/>
+    <sheet name="random_gen_bonus" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="21">
   <si>
     <t>EA</t>
   </si>
@@ -80,11 +83,20 @@
   <si>
     <t>t Critical two-tail</t>
   </si>
+  <si>
+    <t>Uniform Random</t>
+  </si>
+  <si>
+    <t>Validity Enforced Uniform Random</t>
+  </si>
+  <si>
+    <t>t-Test: Two-Sample Assuming Unequal Variances</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -462,11 +474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1315,4 +1327,851 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB6F44F-4A35-4A9F-9268-A260FC822F45}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B2">
+        <v>0.99324324324324298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B4">
+        <v>0.99324324324324298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="B5">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="B6">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.99234234234234187</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.99301801801801781</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B7">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4.6388420106966891E-5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4.2452750980247131E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B8">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B9">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.0927070457354104</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.40647103525242995</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.8608114354760765</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B13">
+        <v>0.97972972972972905</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B14">
+        <v>0.99324324324324298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B16">
+        <v>0.99324324324324298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B18">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.99234234234234187</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.99301801801801781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4.6388420106966891E-5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4.2452750980247131E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B20">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="B22">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1">
+        <v>58</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-0.39263749891266242</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.97297297297297303</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.34801327526618359</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.671552762454859</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.98648648648648596</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.69602655053236717</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0.97297297297297303</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.0017174841452352</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0.97972972972972905</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B29">
+        <v>0.98648648648648596</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.99324324324324298</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>0.99324324324324298</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79374C1-F3BB-4C43-BC08-FFC93D7A54F7}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.990291262135922</v>
+      </c>
+      <c r="B2">
+        <v>0.98989898989898994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.98958333333333304</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.97938144329896903</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.96842105263157896</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.97029702970297005</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.993649068248175</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.99047088971251929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0.99038461538461497</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8.1808938781770772E-5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.0677462196799389E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0.990291262135922</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.979797979797979</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.98958333333333304</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.76618336149476907</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.98850574712643602</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.23887254899478605</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.53739996484069152</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.98823529411764699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0.96808510638297796</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>0.98913043478260798</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>0.98</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.99364906824817545</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.99047088971251929</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>8.1808938781770772E-5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.0677462196799389E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0.98979591836734604</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.98969072164948402</v>
+      </c>
+      <c r="B21">
+        <v>0.96969696969696895</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.98913043478260798</v>
+      </c>
+      <c r="B22">
+        <v>0.97938144329896903</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1">
+        <v>57</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.98019801980197996</v>
+      </c>
+      <c r="B23">
+        <v>0.98</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.2676139262737807</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.98958333333333304</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.10504494312318384</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.98876404494381998</v>
+      </c>
+      <c r="B25">
+        <v>0.99009900990098998</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.6720288884609551</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.978494623655914</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.21008988624636768</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0.97701149425287304</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.0024654592910065</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0.98947368421052595</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>0.98039215686274495</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>